<commit_message>
Add Gmail automation and enhance sentiment analysis
Major features:
- Gmail API integration for automated email fetching
- Automated processor runs every 5 minutes
- Enhanced sentiment analysis with 3 categories (Positive/Negative/Neutral)
- Expanded giving status detection (5 categories)
- Advanced email filtering (admin, parent, technical support, event inquiries)
- Google Sheets monthly worksheet support (jan 2026)
- Chronological email sorting (oldest first)

New files:
- gmail_auth.py: Gmail OAuth authentication
- gmail_to_sheets.py: Main Gmail processing pipeline
- gmail_auto_processor.py: Continuous 5-minute automation
- GMAIL_SETUP.md: Setup documentation

Updated files:
- email_brain.py: Enhanced giving status detection with detailed keywords
- only_filter.py: Added parent, technical support, and event inquiry filters
- sheets_uploader.py: Support for custom worksheet names

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Alumni_Feedback_Report_Filtered.xlsx
+++ b/Alumni_Feedback_Report_Filtered.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,28 +506,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sarah.j@gmail.com</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-10</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>I've been trying to donate on your website for 20 minutes but it keeps crashing. Can someone call me?</t>
+          <t>Thank you so much for the scholarship! It changed my life and I'm forever grateful. I couldn't have finished my degree without this support.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -537,37 +545,41 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chen</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>mchen@yahoo.com</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Thank you so much for the scholarship! It changed my life and I'm forever grateful.</t>
+          <t>I'm extremely disappointed with how the recent fundraising event was handled. The venue was overcrowded and there wasn't enough seating. Very unprofessional.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -577,37 +589,41 @@
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Emily</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rodriguez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>emily.r@outlook.com</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-11</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>I'm interested in making a monthly donation. What are my options?</t>
+          <t>I'm really concerned about the new policy regarding alumni data privacy. I don't feel comfortable with how my information is being shared. This worries me a lot.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -617,37 +633,41 @@
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Thompson</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dthompson@tcnj.edu</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-11</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Please cancel my monthly donation effective immediately.</t>
+          <t>The campus visit last month was absolutely wonderful! Seeing the new library brought back so many memories. I'm so proud of how the school has grown and I'm excited to stay involved.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -657,18 +677,26 @@
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Jessica</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>jwilliams@hotmail.com</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>Negative</t>
@@ -677,38 +705,42 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-11</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>I'm unhappy with the direction you're taking, but I'll continue my monthly donation.</t>
+          <t>I've been a donor for 15 years but after seeing how you treated the faculty during the strike, I'm deeply troubled. This isn't the institution I remember and loved.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Amanda</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ataylor@icloud.com</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>Positive</t>
@@ -717,17 +749,13 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
+          <t>2025-01-12</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Can you help me increase my donation to $100 per month?</t>
+          <t>Just wanted to say thank you for all the amazing work you do in the community! The mentorship program has been wonderful and I'm so proud to be an alum.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -737,13 +765,845 @@
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Christopher</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>chris.lee@company.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-01-12</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>I'm frustrated with the lack of transparency around the budget cuts. Alumni deserve to know what's happening with our donations. This is very concerning to me.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>lisa.a@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>The homecoming celebration was fantastic! I reconnected with so many old friends and the new student center is beautiful. What a great weekend!</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>jgarcia@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>I disagree strongly with the decision to eliminate the arts program. This was always such an important part of campus life and I'm very disappointed by this choice.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Karen</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clark</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>kclark@icloud.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-01-14</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>After this experience with your staff, I will no longer be supporting the annual fund. However, I'll continue my scholarship endowment because I believe in helping students.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Brian</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Lewis</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>blewis@company.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-01-14</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>I'm unhappy with the direction you're taking with the new initiatives, but I'll continue my monthly donation of $100 because I still believe in the mission.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kevin</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Hall</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>khall@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-01-15</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>I'm concerned about the lack of diversity initiatives on campus. We need to do better and I'm worried we're falling behind other schools in this critical area.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>King</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sking@gmail.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>The sustainability efforts on campus are impressive! I love seeing the solar panels and the commitment to reducing carbon emissions. This makes me proud to support the school.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Angela</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Wright</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>awright@icloud.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>I'm deeply upset about how the Title IX investigation was handled. Survivors deserve better and this response was inadequate. I expected more from this institution.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Thomas</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Lopez</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>tlopez@company.com</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>I absolutely love the new alumni magazine! The articles are so well-written and it's wonderful to stay connected with what's happening on campus. Keep up the great work!</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Patricia</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Moore</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>pmoore@gmail.com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>The recent tuition increase is outrageous and puts higher education further out of reach for working families. I'm really disappointed by this decision and the lack of justification.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Gregory</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Martinez</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>gmartinez@yahoo.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Thank you for hosting such a wonderful reunion! It was incredible to see everyone after all these years. The event was perfectly organized and I had an amazing time.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Jennifer</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>jtaylor@outlook.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>I'm thrilled about the new STEM building! This investment in science education is exactly what we need. I'm excited to contribute to this important project.</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Anderson</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>wanderson@gmail.com</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-01-18</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>The treatment of adjunct faculty is shameful and doesn't align with the values this institution claims to uphold. I'm very concerned about this ongoing issue.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Elizabeth</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Thomas</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ethomas@icloud.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-01-18</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>I appreciate all the hard work that went into the capital campaign. The results speak for themselves and I'm proud to have been part of this effort!</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Jackson</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>rjackson@company.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-01-18</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Your response to student mental health concerns has been inadequate. More resources are desperately needed and I'm worried about the wellbeing of current students.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Harris</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>charris@gmail.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-01-19</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>I'm troubled by the lack of support for student activism on campus. Free speech and civic engagement should be encouraged, not suppressed. This concerns me greatly.</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Linda</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>lmartin@outlook.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-01-19</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>The volunteer day was such a rewarding experience! Working alongside current students to give back to the community reminded me why I love being part of this alumni network.</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Thompson</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>jthompson@icloud.com</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-01-20</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>After reading about the financial mismanagement, I've lost confidence in the administration. Better oversight and accountability are urgently needed.</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Barbara</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Garcia</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>bgarcia@gmail.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-01-20</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>The improvements to campus facilities are remarkable! The investment in infrastructure shows a real commitment to providing students with the best possible environment.</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>